<commit_message>
Update .gitignore to exclude Results
</commit_message>
<xml_diff>
--- a/Common_Data/toyKFmodelData8c_locs.xlsx
+++ b/Common_Data/toyKFmodelData8c_locs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JohnMatthew/Downloads/Thorne_15_codefigurestats/Common_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF4F89F-6BEE-F547-8364-878B3DFF2C64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{99F38D23-7719-7347-A416-CC6475B68537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="1280" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2300" yWindow="4260" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="toyKFmodelData8c" sheetId="1" r:id="rId1"/>
@@ -44,6 +44,7 @@
     <definedName name="solver_ver" localSheetId="0" hidden="1">2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -2791,8 +2792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:GL194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" zoomScale="109" workbookViewId="0">
-      <selection activeCell="E112" sqref="E112"/>
+    <sheetView tabSelected="1" topLeftCell="A171" zoomScale="109" workbookViewId="0">
+      <selection activeCell="C179" sqref="C179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12631,7 +12632,7 @@
         <v>478.65002999999996</v>
       </c>
       <c r="G171">
-        <f t="shared" ref="G171:G174" si="18">G$185</f>
+        <f>G$185</f>
         <v>25.176031699999999</v>
       </c>
       <c r="H171">
@@ -12686,7 +12687,7 @@
         <v>496.20003999999994</v>
       </c>
       <c r="G172">
-        <f t="shared" si="18"/>
+        <f>G$185</f>
         <v>25.176031699999999</v>
       </c>
       <c r="H172">
@@ -12741,7 +12742,7 @@
         <v>505.32001999999994</v>
       </c>
       <c r="G173">
-        <f t="shared" si="18"/>
+        <f>G$185</f>
         <v>25.176031699999999</v>
       </c>
       <c r="H173">
@@ -12798,7 +12799,7 @@
         <v>514.45002999999997</v>
       </c>
       <c r="G174">
-        <f t="shared" si="18"/>
+        <f>G$185</f>
         <v>25.176031699999999</v>
       </c>
       <c r="H174">
@@ -13260,15 +13261,15 @@
     </row>
     <row r="193" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C193">
-        <f t="shared" ref="C193:H193" si="19">MIN(C2:C174)</f>
+        <f t="shared" ref="C193:H193" si="18">MIN(C2:C174)</f>
         <v>287.93133230000001</v>
       </c>
       <c r="D193">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.2</v>
       </c>
       <c r="H193">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>-1.0928126309999999</v>
       </c>
       <c r="I193">
@@ -13278,15 +13279,15 @@
     </row>
     <row r="194" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C194">
-        <f t="shared" ref="C194:H194" si="20">MAX(C2:C174)</f>
+        <f t="shared" ref="C194:H194" si="19">MAX(C2:C174)</f>
         <v>563.43971785754434</v>
       </c>
       <c r="D194">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>142.90833330000001</v>
       </c>
       <c r="H194">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>-5.5636842999999998E-2</v>
       </c>
       <c r="I194">

</xml_diff>

<commit_message>
histens fixes, pushing to run LOO code
</commit_message>
<xml_diff>
--- a/Common_Data/toyKFmodelData8c_locs.xlsx
+++ b/Common_Data/toyKFmodelData8c_locs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JohnMatthew/Downloads/Thorne_15_codefigurestats/Common_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{99F38D23-7719-7347-A416-CC6475B68537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21EC3D7C-D50B-0D4A-8A6D-9471D428470C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2300" yWindow="4260" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14380" yWindow="1340" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="toyKFmodelData8c" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,6 @@
     <definedName name="solver_ver" localSheetId="0" hidden="1">2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -84,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="55">
   <si>
     <t>GMST</t>
   </si>
@@ -288,6 +287,9 @@
   </si>
   <si>
     <t>Raw area average</t>
+  </si>
+  <si>
+    <t>change</t>
   </si>
 </sst>
 </file>
@@ -2792,8 +2794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:GL194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A171" zoomScale="109" workbookViewId="0">
-      <selection activeCell="C179" sqref="C179"/>
+    <sheetView tabSelected="1" topLeftCell="A159" zoomScale="109" workbookViewId="0">
+      <selection activeCell="K185" sqref="K185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4531,7 +4533,7 @@
         <v>2005.5</v>
       </c>
       <c r="W23">
-        <f t="shared" ref="W23:AN23" si="2">V23+1</f>
+        <f t="shared" ref="W23:AO23" si="2">V23+1</f>
         <v>2006.5</v>
       </c>
       <c r="X23">
@@ -4602,6 +4604,10 @@
         <f t="shared" si="2"/>
         <v>2023.5</v>
       </c>
+      <c r="AO23">
+        <f t="shared" si="2"/>
+        <v>2024.5</v>
+      </c>
     </row>
     <row r="24" spans="1:169" x14ac:dyDescent="0.2">
       <c r="A24">
@@ -4634,10 +4640,10 @@
       <c r="Q24">
         <v>288.2</v>
       </c>
-      <c r="T24" t="s">
+      <c r="T24" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="U24" t="s">
+      <c r="U24" s="2" t="s">
         <v>19</v>
       </c>
       <c r="V24">
@@ -4695,7 +4701,10 @@
         <v>28.191998999999999</v>
       </c>
       <c r="AN24">
-        <v>29.105</v>
+        <v>29.22</v>
+      </c>
+      <c r="AO24">
+        <v>30.315999999999999</v>
       </c>
     </row>
     <row r="25" spans="1:169" x14ac:dyDescent="0.2">
@@ -4729,6 +4738,9 @@
       <c r="Q25">
         <v>288.39999999999998</v>
       </c>
+      <c r="U25" t="s">
+        <v>54</v>
+      </c>
       <c r="V25">
         <f t="shared" ref="V25:AM25" si="3">(W24-V24)*10</f>
         <v>24.670000000000005</v>
@@ -4786,7 +4798,7 @@
         <v>13.770009999999999</v>
       </c>
       <c r="AJ25">
-        <f t="shared" si="3"/>
+        <f>(AK24-AJ24)*10</f>
         <v>0.88998999999997608</v>
       </c>
       <c r="AK25">
@@ -4799,7 +4811,11 @@
       </c>
       <c r="AM25">
         <f t="shared" si="3"/>
-        <v>9.1300100000000128</v>
+        <v>10.280009999999997</v>
+      </c>
+      <c r="AN25">
+        <f t="shared" ref="AN25" si="4">(AO24-AN24)*10</f>
+        <v>10.96</v>
       </c>
     </row>
     <row r="26" spans="1:169" x14ac:dyDescent="0.2">
@@ -4866,79 +4882,79 @@
         <v>288.7</v>
       </c>
       <c r="V27">
-        <f t="shared" ref="V27:AN27" si="4">EZ17</f>
+        <f t="shared" ref="V27:AN27" si="5">EZ17</f>
         <v>2005</v>
       </c>
       <c r="W27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2006</v>
       </c>
       <c r="X27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2007</v>
       </c>
       <c r="Y27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2008</v>
       </c>
       <c r="Z27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2009</v>
       </c>
       <c r="AA27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2010</v>
       </c>
       <c r="AB27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2011</v>
       </c>
       <c r="AC27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2012</v>
       </c>
       <c r="AD27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2013</v>
       </c>
       <c r="AE27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2014</v>
       </c>
       <c r="AF27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2015</v>
       </c>
       <c r="AG27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2016</v>
       </c>
       <c r="AH27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2017</v>
       </c>
       <c r="AI27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2018</v>
       </c>
       <c r="AJ27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AK27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AL27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AM27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AN27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -4977,59 +4993,59 @@
         <v>24</v>
       </c>
       <c r="V28">
-        <f t="shared" ref="V28:AI28" si="5">EZ18</f>
+        <f t="shared" ref="V28:AI28" si="6">EZ18</f>
         <v>385.509615</v>
       </c>
       <c r="W28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>389.38556799999998</v>
       </c>
       <c r="X28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>391.97981600000003</v>
       </c>
       <c r="Y28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>395.58442400000001</v>
       </c>
       <c r="Z28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>399.40767099999999</v>
       </c>
       <c r="AA28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>403.10555199999999</v>
       </c>
       <c r="AB28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>409.976023</v>
       </c>
       <c r="AC28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>417.51569899999998</v>
       </c>
       <c r="AD28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>425.15174400000001</v>
       </c>
       <c r="AE28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>433.95852500000001</v>
       </c>
       <c r="AF28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>444.16807799999998</v>
       </c>
       <c r="AG28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>453.15947499999999</v>
       </c>
       <c r="AH28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>460.30364900000001</v>
       </c>
       <c r="AI28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>463.99002999999999</v>
       </c>
       <c r="AJ28">
@@ -5050,7 +5066,7 @@
       </c>
       <c r="AN28">
         <f>AM28+AM33</f>
-        <v>514.45002999999997</v>
+        <v>515.60002999999995</v>
       </c>
     </row>
     <row r="29" spans="1:169" x14ac:dyDescent="0.2">
@@ -5085,55 +5101,55 @@
         <v>289.5</v>
       </c>
       <c r="V29">
-        <f t="shared" ref="V29:AH29" si="6">W28-V28</f>
+        <f t="shared" ref="V29:AH29" si="7">W28-V28</f>
         <v>3.8759529999999813</v>
       </c>
       <c r="W29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.5942480000000501</v>
       </c>
       <c r="X29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.6046079999999847</v>
       </c>
       <c r="Y29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.8232469999999807</v>
       </c>
       <c r="Z29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.6978809999999953</v>
       </c>
       <c r="AA29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6.8704710000000091</v>
       </c>
       <c r="AB29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7.5396759999999858</v>
       </c>
       <c r="AC29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7.6360450000000242</v>
       </c>
       <c r="AD29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>8.8067810000000009</v>
       </c>
       <c r="AE29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10.209552999999971</v>
       </c>
       <c r="AF29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>8.9913970000000063</v>
       </c>
       <c r="AG29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7.1441740000000209</v>
       </c>
       <c r="AH29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.686380999999983</v>
       </c>
     </row>
@@ -5289,7 +5305,11 @@
       </c>
       <c r="AM33">
         <f>AM25</f>
-        <v>9.1300100000000128</v>
+        <v>10.280009999999997</v>
+      </c>
+      <c r="AN33">
+        <f>AN25</f>
+        <v>10.96</v>
       </c>
     </row>
     <row r="34" spans="1:194" x14ac:dyDescent="0.2">
@@ -5380,7 +5400,7 @@
       </c>
       <c r="AM35">
         <f>AN36-AM36</f>
-        <v>-509.30325370000003</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:194" x14ac:dyDescent="0.2">
@@ -5434,6 +5454,9 @@
       <c r="AM36">
         <v>509.30325370000003</v>
       </c>
+      <c r="AN36">
+        <v>510.30325370000003</v>
+      </c>
     </row>
     <row r="37" spans="1:194" x14ac:dyDescent="0.2">
       <c r="A37">
@@ -5566,695 +5589,695 @@
         <v>1850</v>
       </c>
       <c r="V40">
-        <f t="shared" ref="V40:BA40" si="7">U40+1</f>
+        <f t="shared" ref="V40:BA40" si="8">U40+1</f>
         <v>1851</v>
       </c>
       <c r="W40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1852</v>
       </c>
       <c r="X40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1853</v>
       </c>
       <c r="Y40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1854</v>
       </c>
       <c r="Z40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1855</v>
       </c>
       <c r="AA40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1856</v>
       </c>
       <c r="AB40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1857</v>
       </c>
       <c r="AC40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1858</v>
       </c>
       <c r="AD40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1859</v>
       </c>
       <c r="AE40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1860</v>
       </c>
       <c r="AF40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1861</v>
       </c>
       <c r="AG40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1862</v>
       </c>
       <c r="AH40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1863</v>
       </c>
       <c r="AI40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1864</v>
       </c>
       <c r="AJ40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1865</v>
       </c>
       <c r="AK40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1866</v>
       </c>
       <c r="AL40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1867</v>
       </c>
       <c r="AM40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1868</v>
       </c>
       <c r="AN40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1869</v>
       </c>
       <c r="AO40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1870</v>
       </c>
       <c r="AP40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1871</v>
       </c>
       <c r="AQ40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1872</v>
       </c>
       <c r="AR40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1873</v>
       </c>
       <c r="AS40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1874</v>
       </c>
       <c r="AT40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1875</v>
       </c>
       <c r="AU40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1876</v>
       </c>
       <c r="AV40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1877</v>
       </c>
       <c r="AW40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1878</v>
       </c>
       <c r="AX40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1879</v>
       </c>
       <c r="AY40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1880</v>
       </c>
       <c r="AZ40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1881</v>
       </c>
       <c r="BA40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1882</v>
       </c>
       <c r="BB40">
-        <f t="shared" ref="BB40:CG40" si="8">BA40+1</f>
+        <f t="shared" ref="BB40:CG40" si="9">BA40+1</f>
         <v>1883</v>
       </c>
       <c r="BC40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1884</v>
       </c>
       <c r="BD40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1885</v>
       </c>
       <c r="BE40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1886</v>
       </c>
       <c r="BF40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1887</v>
       </c>
       <c r="BG40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1888</v>
       </c>
       <c r="BH40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1889</v>
       </c>
       <c r="BI40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1890</v>
       </c>
       <c r="BJ40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1891</v>
       </c>
       <c r="BK40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1892</v>
       </c>
       <c r="BL40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1893</v>
       </c>
       <c r="BM40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1894</v>
       </c>
       <c r="BN40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1895</v>
       </c>
       <c r="BO40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1896</v>
       </c>
       <c r="BP40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1897</v>
       </c>
       <c r="BQ40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1898</v>
       </c>
       <c r="BR40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1899</v>
       </c>
       <c r="BS40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1900</v>
       </c>
       <c r="BT40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1901</v>
       </c>
       <c r="BU40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1902</v>
       </c>
       <c r="BV40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1903</v>
       </c>
       <c r="BW40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1904</v>
       </c>
       <c r="BX40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1905</v>
       </c>
       <c r="BY40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1906</v>
       </c>
       <c r="BZ40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1907</v>
       </c>
       <c r="CA40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1908</v>
       </c>
       <c r="CB40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1909</v>
       </c>
       <c r="CC40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1910</v>
       </c>
       <c r="CD40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1911</v>
       </c>
       <c r="CE40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1912</v>
       </c>
       <c r="CF40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1913</v>
       </c>
       <c r="CG40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1914</v>
       </c>
       <c r="CH40">
-        <f t="shared" ref="CH40:DM40" si="9">CG40+1</f>
+        <f t="shared" ref="CH40:DM40" si="10">CG40+1</f>
         <v>1915</v>
       </c>
       <c r="CI40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1916</v>
       </c>
       <c r="CJ40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1917</v>
       </c>
       <c r="CK40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1918</v>
       </c>
       <c r="CL40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1919</v>
       </c>
       <c r="CM40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1920</v>
       </c>
       <c r="CN40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1921</v>
       </c>
       <c r="CO40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1922</v>
       </c>
       <c r="CP40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1923</v>
       </c>
       <c r="CQ40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1924</v>
       </c>
       <c r="CR40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1925</v>
       </c>
       <c r="CS40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1926</v>
       </c>
       <c r="CT40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1927</v>
       </c>
       <c r="CU40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1928</v>
       </c>
       <c r="CV40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1929</v>
       </c>
       <c r="CW40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1930</v>
       </c>
       <c r="CX40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1931</v>
       </c>
       <c r="CY40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1932</v>
       </c>
       <c r="CZ40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1933</v>
       </c>
       <c r="DA40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1934</v>
       </c>
       <c r="DB40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1935</v>
       </c>
       <c r="DC40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1936</v>
       </c>
       <c r="DD40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1937</v>
       </c>
       <c r="DE40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1938</v>
       </c>
       <c r="DF40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1939</v>
       </c>
       <c r="DG40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1940</v>
       </c>
       <c r="DH40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1941</v>
       </c>
       <c r="DI40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1942</v>
       </c>
       <c r="DJ40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1943</v>
       </c>
       <c r="DK40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1944</v>
       </c>
       <c r="DL40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1945</v>
       </c>
       <c r="DM40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1946</v>
       </c>
       <c r="DN40">
-        <f t="shared" ref="DN40:ES40" si="10">DM40+1</f>
+        <f t="shared" ref="DN40:ES40" si="11">DM40+1</f>
         <v>1947</v>
       </c>
       <c r="DO40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1948</v>
       </c>
       <c r="DP40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1949</v>
       </c>
       <c r="DQ40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1950</v>
       </c>
       <c r="DR40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1951</v>
       </c>
       <c r="DS40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1952</v>
       </c>
       <c r="DT40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1953</v>
       </c>
       <c r="DU40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1954</v>
       </c>
       <c r="DV40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1955</v>
       </c>
       <c r="DW40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1956</v>
       </c>
       <c r="DX40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1957</v>
       </c>
       <c r="DY40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1958</v>
       </c>
       <c r="DZ40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1959</v>
       </c>
       <c r="EA40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1960</v>
       </c>
       <c r="EB40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1961</v>
       </c>
       <c r="EC40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1962</v>
       </c>
       <c r="ED40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1963</v>
       </c>
       <c r="EE40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1964</v>
       </c>
       <c r="EF40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1965</v>
       </c>
       <c r="EG40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1966</v>
       </c>
       <c r="EH40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1967</v>
       </c>
       <c r="EI40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1968</v>
       </c>
       <c r="EJ40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1969</v>
       </c>
       <c r="EK40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1970</v>
       </c>
       <c r="EL40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1971</v>
       </c>
       <c r="EM40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1972</v>
       </c>
       <c r="EN40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1973</v>
       </c>
       <c r="EO40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1974</v>
       </c>
       <c r="EP40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1975</v>
       </c>
       <c r="EQ40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1976</v>
       </c>
       <c r="ER40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1977</v>
       </c>
       <c r="ES40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1978</v>
       </c>
       <c r="ET40">
-        <f t="shared" ref="ET40:FY40" si="11">ES40+1</f>
+        <f t="shared" ref="ET40:FY40" si="12">ES40+1</f>
         <v>1979</v>
       </c>
       <c r="EU40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1980</v>
       </c>
       <c r="EV40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1981</v>
       </c>
       <c r="EW40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1982</v>
       </c>
       <c r="EX40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1983</v>
       </c>
       <c r="EY40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1984</v>
       </c>
       <c r="EZ40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1985</v>
       </c>
       <c r="FA40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1986</v>
       </c>
       <c r="FB40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1987</v>
       </c>
       <c r="FC40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1988</v>
       </c>
       <c r="FD40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1989</v>
       </c>
       <c r="FE40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1990</v>
       </c>
       <c r="FF40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1991</v>
       </c>
       <c r="FG40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1992</v>
       </c>
       <c r="FH40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1993</v>
       </c>
       <c r="FI40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1994</v>
       </c>
       <c r="FJ40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1995</v>
       </c>
       <c r="FK40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1996</v>
       </c>
       <c r="FL40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1997</v>
       </c>
       <c r="FM40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1998</v>
       </c>
       <c r="FN40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1999</v>
       </c>
       <c r="FO40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2000</v>
       </c>
       <c r="FP40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2001</v>
       </c>
       <c r="FQ40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2002</v>
       </c>
       <c r="FR40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2003</v>
       </c>
       <c r="FS40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2004</v>
       </c>
       <c r="FT40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2005</v>
       </c>
       <c r="FU40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2006</v>
       </c>
       <c r="FV40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2007</v>
       </c>
       <c r="FW40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2008</v>
       </c>
       <c r="FX40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2009</v>
       </c>
       <c r="FY40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2010</v>
       </c>
       <c r="FZ40">
-        <f t="shared" ref="FZ40:GL40" si="12">FY40+1</f>
+        <f t="shared" ref="FZ40:GL40" si="13">FY40+1</f>
         <v>2011</v>
       </c>
       <c r="GA40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2012</v>
       </c>
       <c r="GB40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2013</v>
       </c>
       <c r="GC40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2014</v>
       </c>
       <c r="GD40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2015</v>
       </c>
       <c r="GE40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2016</v>
       </c>
       <c r="GF40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2017</v>
       </c>
       <c r="GG40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2018</v>
       </c>
       <c r="GH40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2019</v>
       </c>
       <c r="GI40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2020</v>
       </c>
       <c r="GJ40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2021</v>
       </c>
       <c r="GK40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2022</v>
       </c>
       <c r="GL40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2023</v>
       </c>
     </row>
@@ -7330,7 +7353,7 @@
         <v>9.1919091031583203E-2</v>
       </c>
       <c r="K53" s="8">
-        <f t="shared" ref="K53:K76" si="13">(J53-$J$81)*$K$81</f>
+        <f t="shared" ref="K53:K76" si="14">(J53-$J$81)*$K$81</f>
         <v>52.56878694989161</v>
       </c>
       <c r="O53" s="7">
@@ -7375,7 +7398,7 @@
         <v>9.68285181566544E-2</v>
       </c>
       <c r="K54" s="8">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>60.11692635106418</v>
       </c>
       <c r="O54" s="7">
@@ -7420,7 +7443,7 @@
         <v>7.4245710810314197E-2</v>
       </c>
       <c r="K55" s="8">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>25.39634214083868</v>
       </c>
       <c r="O55" s="7">
@@ -7465,7 +7488,7 @@
         <v>6.6449448478761206E-2</v>
       </c>
       <c r="K56" s="8">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>13.409755236196679</v>
       </c>
       <c r="O56" s="7">
@@ -7510,7 +7533,7 @@
         <v>6.6743266192952497E-2</v>
       </c>
       <c r="K57" s="8">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>13.861493699514348</v>
       </c>
       <c r="O57" s="7">
@@ -7555,7 +7578,7 @@
         <v>6.5304095541377394E-2</v>
       </c>
       <c r="K58" s="8">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>11.64879954530431</v>
       </c>
       <c r="O58" s="7">
@@ -7600,7 +7623,7 @@
         <v>6.4138285976007695E-2</v>
       </c>
       <c r="K59" s="8">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>9.8563922255799596</v>
       </c>
       <c r="O59" s="7">
@@ -7645,7 +7668,7 @@
         <v>6.3111068768934103E-2</v>
       </c>
       <c r="K60" s="8">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>8.2770676981459825</v>
       </c>
       <c r="O60" s="7">
@@ -7690,7 +7713,7 @@
         <v>6.3649044853189896E-2</v>
       </c>
       <c r="K61" s="8">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>9.1041944432854756</v>
       </c>
       <c r="O61" s="7">
@@ -7735,7 +7758,7 @@
         <v>9.4999905151178995E-2</v>
       </c>
       <c r="K62" s="8">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>57.305472891323632</v>
       </c>
       <c r="O62" s="7">
@@ -7780,7 +7803,7 @@
         <v>0.119516241543702</v>
       </c>
       <c r="K63" s="8">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>94.998816734190044</v>
       </c>
       <c r="O63" s="7">
@@ -7825,7 +7848,7 @@
         <v>8.3136715299136799E-2</v>
       </c>
       <c r="K64" s="8">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>39.066071742357266</v>
       </c>
       <c r="O64" s="7">
@@ -7870,7 +7893,7 @@
         <v>7.00512777491889E-2</v>
       </c>
       <c r="K65" s="8">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>18.947490849701207</v>
       </c>
       <c r="O65" s="7">
@@ -7915,7 +7938,7 @@
         <v>6.4197988756666199E-2</v>
       </c>
       <c r="K66" s="8">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>9.9481839763418147</v>
       </c>
       <c r="O66" s="7">
@@ -7960,7 +7983,7 @@
         <v>6.2550100482268403E-2</v>
       </c>
       <c r="K67" s="8">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>7.4145909326255595</v>
       </c>
       <c r="O67" s="7">
@@ -8005,7 +8028,7 @@
         <v>6.1754841581801598E-2</v>
       </c>
       <c r="K68" s="8">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>6.1918973498871024</v>
       </c>
       <c r="O68" s="7">
@@ -8050,7 +8073,7 @@
         <v>5.9625417147255597E-2</v>
       </c>
       <c r="K69" s="8">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2.9179527394997571</v>
       </c>
       <c r="O69" s="7">
@@ -8095,7 +8118,7 @@
         <v>5.97054454026439E-2</v>
       </c>
       <c r="K70" s="8">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3.0409944737621424</v>
       </c>
       <c r="O70" s="7">
@@ -8140,7 +8163,7 @@
         <v>6.04255483036025E-2</v>
       </c>
       <c r="K71" s="8">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>4.148137311643751</v>
       </c>
       <c r="O71" s="7">
@@ -8185,7 +8208,7 @@
         <v>5.9266397915716397E-2</v>
       </c>
       <c r="K72" s="8">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2.3659683351441414</v>
       </c>
       <c r="O72" s="7">
@@ -8230,7 +8253,7 @@
         <v>5.9624377481728101E-2</v>
       </c>
       <c r="K73" s="8">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2.9163542759454142</v>
       </c>
       <c r="O73" s="7">
@@ -8275,7 +8298,7 @@
         <v>5.9728054106763198E-2</v>
       </c>
       <c r="K74" s="8">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3.075754873707961</v>
       </c>
       <c r="O74" s="7">
@@ -8320,7 +8343,7 @@
         <v>5.9253809334799998E-2</v>
       </c>
       <c r="K75" s="8">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2.3466136607189569</v>
       </c>
       <c r="O75" s="7">
@@ -8365,7 +8388,7 @@
         <v>6.0520394452817303E-2</v>
       </c>
       <c r="K76" s="8">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>4.2939612413405106</v>
       </c>
       <c r="O76" s="7">
@@ -9143,7 +9166,7 @@
         <v>340.23529050000002</v>
       </c>
       <c r="J96" s="8">
-        <f t="shared" ref="J96:J108" si="14">J131/2+65</f>
+        <f t="shared" ref="J96:J108" si="15">J131/2+65</f>
         <v>67.230560288547636</v>
       </c>
       <c r="K96" s="8">
@@ -9189,11 +9212,11 @@
         <v>340.27209475000001</v>
       </c>
       <c r="J97" s="8">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>67.178497181698333</v>
       </c>
       <c r="K97" s="8">
-        <f t="shared" ref="K97:K121" si="15">(J97-$J$126)*$K$126</f>
+        <f t="shared" ref="K97:K121" si="16">(J97-$J$126)*$K$126</f>
         <v>6.0383590534773708</v>
       </c>
       <c r="O97" s="7">
@@ -9235,11 +9258,11 @@
         <v>340.34817500000003</v>
       </c>
       <c r="J98" s="8">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>102.4396720880046</v>
       </c>
       <c r="K98" s="8">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>55.768729709188577</v>
       </c>
       <c r="O98" s="7">
@@ -9281,11 +9304,11 @@
         <v>340.37658699999997</v>
       </c>
       <c r="J99" s="8">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>105.0094489597104</v>
       </c>
       <c r="K99" s="8">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>59.392997949596747</v>
       </c>
       <c r="O99" s="7">
@@ -9327,11 +9350,11 @@
         <v>340.35220325</v>
       </c>
       <c r="J100" s="8">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>80.48010903873265</v>
       </c>
       <c r="K100" s="8">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>24.798201563728355</v>
       </c>
       <c r="O100" s="7">
@@ -9373,11 +9396,11 @@
         <v>340.27947999999998</v>
       </c>
       <c r="J101" s="8">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>71.657119258458295</v>
       </c>
       <c r="K101" s="8">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>12.354754820094072</v>
       </c>
       <c r="O101" s="7">
@@ -9419,11 +9442,11 @@
         <v>340.21243275</v>
       </c>
       <c r="J102" s="8">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>72.517050724503406</v>
       </c>
       <c r="K102" s="8">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>13.567553618164874</v>
       </c>
       <c r="O102" s="7">
@@ -9465,11 +9488,11 @@
         <v>340.20559700000001</v>
       </c>
       <c r="J103" s="8">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>70.871736280776247</v>
       </c>
       <c r="K103" s="8">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>11.247095001877716</v>
       </c>
       <c r="O103" s="7">
@@ -9511,11 +9534,11 @@
         <v>340.17346199999997</v>
       </c>
       <c r="J104" s="8">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>69.566575546913256</v>
       </c>
       <c r="K104" s="8">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>9.4063699768962454</v>
       </c>
       <c r="O104" s="7">
@@ -9557,11 +9580,11 @@
         <v>340.17523199999999</v>
       </c>
       <c r="J105" s="8">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>68.483122325627306</v>
       </c>
       <c r="K105" s="8">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>7.8783287126490249</v>
       </c>
       <c r="O105" s="7">
@@ -9603,11 +9626,11 @@
         <v>340.22027600000001</v>
       </c>
       <c r="J106" s="8">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>69.398758094648031</v>
       </c>
       <c r="K106" s="8">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>9.1696897152253776</v>
       </c>
       <c r="O106" s="7">
@@ -9649,11 +9672,11 @@
         <v>340.35534675000002</v>
       </c>
       <c r="J107" s="8">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>104.6702341605297</v>
       </c>
       <c r="K107" s="8">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>58.914588544919148</v>
       </c>
       <c r="O107" s="7">
@@ -9695,11 +9718,11 @@
         <v>340.48495474999999</v>
       </c>
       <c r="J108" s="8">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>128.10536110650949</v>
       </c>
       <c r="K108" s="8">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>91.966168717274343</v>
       </c>
       <c r="O108" s="7">
@@ -9741,11 +9764,11 @@
         <v>340.46524049999999</v>
       </c>
       <c r="J109" s="8">
-        <f t="shared" ref="J109:J120" si="16">J144/2+65</f>
+        <f t="shared" ref="J109:J120" si="17">J144/2+65</f>
         <v>89.051117294368709</v>
       </c>
       <c r="K109" s="8">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>36.886267788932649</v>
       </c>
       <c r="O109" s="7">
@@ -9787,11 +9810,11 @@
         <v>340.39031975</v>
       </c>
       <c r="J110" s="8">
+        <f t="shared" si="17"/>
+        <v>76.058780188067345</v>
+      </c>
+      <c r="K110" s="8">
         <f t="shared" si="16"/>
-        <v>76.058780188067345</v>
-      </c>
-      <c r="K110" s="8">
-        <f t="shared" si="15"/>
         <v>18.562608929092352</v>
       </c>
       <c r="L110" s="6">
@@ -9836,11 +9859,11 @@
         <v>340.35687250000001</v>
       </c>
       <c r="J111" s="8">
+        <f t="shared" si="17"/>
+        <v>69.789003483091676</v>
+      </c>
+      <c r="K111" s="8">
         <f t="shared" si="16"/>
-        <v>69.789003483091676</v>
-      </c>
-      <c r="K111" s="8">
-        <f t="shared" si="15"/>
         <v>9.7200697824112172</v>
       </c>
       <c r="L111" s="6">
@@ -9885,11 +9908,11 @@
         <v>340.24893200000002</v>
       </c>
       <c r="J112" s="8">
+        <f t="shared" si="17"/>
+        <v>68.146294608723508</v>
+      </c>
+      <c r="K112" s="8">
         <f t="shared" si="16"/>
-        <v>68.146294608723508</v>
-      </c>
-      <c r="K112" s="8">
-        <f t="shared" si="15"/>
         <v>7.4032859140681104</v>
       </c>
       <c r="L112">
@@ -9934,11 +9957,11 @@
         <v>340.199524</v>
       </c>
       <c r="J113" s="8">
+        <f t="shared" si="17"/>
+        <v>67.492662695167155</v>
+      </c>
+      <c r="K113" s="8">
         <f t="shared" si="16"/>
-        <v>67.492662695167155</v>
-      </c>
-      <c r="K113" s="8">
-        <f t="shared" si="15"/>
         <v>6.4814403595756591</v>
       </c>
       <c r="L113">
@@ -9983,11 +10006,11 @@
         <v>340.18313599999999</v>
       </c>
       <c r="J114" s="8">
+        <f t="shared" si="17"/>
+        <v>65.384801557870745</v>
+      </c>
+      <c r="K114" s="8">
         <f t="shared" si="16"/>
-        <v>65.384801557870745</v>
-      </c>
-      <c r="K114" s="8">
-        <f t="shared" si="15"/>
         <v>3.508631996636733</v>
       </c>
       <c r="L114">
@@ -10032,11 +10055,11 @@
         <v>340.18191524999997</v>
       </c>
       <c r="J115" s="8">
+        <f t="shared" si="17"/>
+        <v>65.566936104019248</v>
+      </c>
+      <c r="K115" s="8">
         <f t="shared" si="16"/>
-        <v>65.566936104019248</v>
-      </c>
-      <c r="K115" s="8">
-        <f t="shared" si="15"/>
         <v>3.7655042793454676</v>
       </c>
       <c r="L115">
@@ -10081,11 +10104,11 @@
         <v>340.193512</v>
       </c>
       <c r="J116" s="8">
+        <f t="shared" si="17"/>
+        <v>66.36734872403828</v>
+      </c>
+      <c r="K116" s="8">
         <f t="shared" si="16"/>
-        <v>66.36734872403828</v>
-      </c>
-      <c r="K116" s="8">
-        <f t="shared" si="15"/>
         <v>4.894361056716674</v>
       </c>
       <c r="L116">
@@ -10130,11 +10153,11 @@
         <v>340.25051875000003</v>
       </c>
       <c r="J117" s="8">
+        <f t="shared" si="17"/>
+        <v>65</v>
+      </c>
+      <c r="K117" s="8">
         <f t="shared" si="16"/>
-        <v>65</v>
-      </c>
-      <c r="K117" s="8">
-        <f t="shared" si="15"/>
         <v>2.9659296007961222</v>
       </c>
       <c r="L117">
@@ -10179,11 +10202,11 @@
         <v>340.30575549999998</v>
       </c>
       <c r="J118" s="8">
+        <f t="shared" si="17"/>
+        <v>65.365352551456851</v>
+      </c>
+      <c r="K118" s="8">
         <f t="shared" si="16"/>
-        <v>65.365352551456851</v>
-      </c>
-      <c r="K118" s="8">
-        <f t="shared" si="15"/>
         <v>3.4812022158532452</v>
       </c>
       <c r="L118">
@@ -10228,11 +10251,11 @@
         <v>340.32592775000001</v>
       </c>
       <c r="J119" s="8">
+        <f t="shared" si="17"/>
+        <v>65.521455750125469</v>
+      </c>
+      <c r="K119" s="8">
         <f t="shared" si="16"/>
-        <v>65.521455750125469</v>
-      </c>
-      <c r="K119" s="8">
-        <f t="shared" si="15"/>
         <v>3.701361355500747</v>
       </c>
       <c r="L119">
@@ -10277,11 +10300,11 @@
         <v>340.34426875000003</v>
       </c>
       <c r="J120" s="8">
+        <f t="shared" si="17"/>
+        <v>65.043471926671813</v>
+      </c>
+      <c r="K120" s="8">
         <f t="shared" si="16"/>
-        <v>65.043471926671813</v>
-      </c>
-      <c r="K120" s="8">
-        <f t="shared" si="15"/>
         <v>3.0272399522592135</v>
       </c>
       <c r="L120">
@@ -10330,7 +10353,7 @@
         <v>66.442674930835111</v>
       </c>
       <c r="K121" s="8">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>5.0005968867492463</v>
       </c>
       <c r="L121">
@@ -11685,7 +11708,7 @@
         <v>0</v>
       </c>
       <c r="K152" s="4">
-        <f t="shared" ref="K152:K173" si="17">C152/M152</f>
+        <f t="shared" ref="K152:K173" si="18">C152/M152</f>
         <v>1.2844127305289239</v>
       </c>
       <c r="L152">
@@ -11733,7 +11756,7 @@
         <v>0.73070510291370305</v>
       </c>
       <c r="K153" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.2896606659526042</v>
       </c>
       <c r="L153">
@@ -11781,7 +11804,7 @@
         <v>1.0429115002509499</v>
       </c>
       <c r="K154" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.292247495345497</v>
       </c>
       <c r="L154">
@@ -11829,7 +11852,7 @@
         <v>8.6943853343623895E-2</v>
       </c>
       <c r="K155" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.2980578035477892</v>
       </c>
       <c r="L155">
@@ -11877,7 +11900,7 @@
         <v>2.88534986167021</v>
       </c>
       <c r="K156" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.3008457668824673</v>
       </c>
       <c r="L156">
@@ -11922,7 +11945,7 @@
         <v>340.16989124999998</v>
       </c>
       <c r="K157" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.303516323641027</v>
       </c>
       <c r="L157">
@@ -11967,7 +11990,7 @@
         <v>340.15097050000003</v>
       </c>
       <c r="K158" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.3074041654080517</v>
       </c>
       <c r="L158">
@@ -12012,7 +12035,7 @@
         <v>340.15243525</v>
       </c>
       <c r="K159" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.3076934554078221</v>
       </c>
       <c r="L159">
@@ -12057,7 +12080,7 @@
         <v>340.15164175000001</v>
       </c>
       <c r="K160" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.3054555136208854</v>
       </c>
       <c r="L160">
@@ -12102,7 +12125,7 @@
         <v>340.19635</v>
       </c>
       <c r="K161" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.3127154619328378</v>
       </c>
       <c r="L161">
@@ -12150,7 +12173,7 @@
         <v>340.26724250000001</v>
       </c>
       <c r="K162" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.3143149677172385</v>
       </c>
       <c r="L162">
@@ -12195,7 +12218,7 @@
         <v>340.29815674999998</v>
       </c>
       <c r="K163" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.3183146043749683</v>
       </c>
       <c r="L163">
@@ -12240,7 +12263,7 @@
         <v>340.3157655</v>
       </c>
       <c r="K164" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.3169033787871149</v>
       </c>
       <c r="L164">
@@ -12297,7 +12320,7 @@
         <v>340.34655750000002</v>
       </c>
       <c r="K165" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.3219506559514553</v>
       </c>
       <c r="L165">
@@ -12354,7 +12377,7 @@
         <v>340.35244749999998</v>
       </c>
       <c r="K166" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.3273215932271014</v>
       </c>
       <c r="L166">
@@ -12411,7 +12434,7 @@
         <v>340.237976</v>
       </c>
       <c r="K167" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.3250198009445859</v>
       </c>
       <c r="L167">
@@ -12468,7 +12491,7 @@
         <v>340.164917</v>
       </c>
       <c r="K168" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.3288625196676174</v>
       </c>
       <c r="L168">
@@ -12525,7 +12548,7 @@
         <v>340.15966800000001</v>
       </c>
       <c r="K169" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.3319322521530632</v>
       </c>
       <c r="L169">
@@ -12584,7 +12607,7 @@
         <v>340.16229249999998</v>
       </c>
       <c r="K170" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.3389050615814406</v>
       </c>
       <c r="L170">
@@ -12642,7 +12665,7 @@
         <v>340.18728650000003</v>
       </c>
       <c r="K171" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.3100757639844525</v>
       </c>
       <c r="L171">
@@ -12697,7 +12720,7 @@
         <v>340.24371350000001</v>
       </c>
       <c r="K172" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.3242324749645782</v>
       </c>
       <c r="L172">
@@ -12752,7 +12775,7 @@
         <v>340.37359624999999</v>
       </c>
       <c r="K173" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.3349507516784938</v>
       </c>
       <c r="L173">
@@ -12796,7 +12819,7 @@
         <v>1.933275000000001E-2</v>
       </c>
       <c r="F174">
-        <v>514.45002999999997</v>
+        <v>515.60002999999995</v>
       </c>
       <c r="G174">
         <f>G$185</f>
@@ -13261,15 +13284,15 @@
     </row>
     <row r="193" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C193">
-        <f t="shared" ref="C193:H193" si="18">MIN(C2:C174)</f>
+        <f t="shared" ref="C193:H193" si="19">MIN(C2:C174)</f>
         <v>287.93133230000001</v>
       </c>
       <c r="D193">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.2</v>
       </c>
       <c r="H193">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>-1.0928126309999999</v>
       </c>
       <c r="I193">
@@ -13279,15 +13302,15 @@
     </row>
     <row r="194" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C194">
-        <f t="shared" ref="C194:H194" si="19">MAX(C2:C174)</f>
+        <f t="shared" ref="C194:H194" si="20">MAX(C2:C174)</f>
         <v>563.43971785754434</v>
       </c>
       <c r="D194">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>142.90833330000001</v>
       </c>
       <c r="H194">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>-5.5636842999999998E-2</v>
       </c>
       <c r="I194">
@@ -13305,8 +13328,10 @@
     <hyperlink ref="D183" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="I178" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="F185" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="T24" r:id="rId6" xr:uid="{3D1A698D-BFFE-0548-A5AF-B93376F1206E}"/>
+    <hyperlink ref="U24" r:id="rId7" xr:uid="{1CD6EC45-3ADE-E748-B37A-82E6011EB91A}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId6"/>
+  <drawing r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>